<commit_message>
Base de datos 2
</commit_message>
<xml_diff>
--- a/ddbb/diccionario_datos.xlsx
+++ b/ddbb/diccionario_datos.xlsx
@@ -1,13 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27004"/>
   <workbookPr/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0453ED16-2495-4225-ABD9-BFE899792768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Hoja1" sheetId="1" r:id="rId4"/>
+    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191028"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="vk3EAQX1I26mcZugeMsWwhJRaDjPYWI2sezbjj3TsLI="/>
     </ext>
@@ -204,7 +222,7 @@
     <t>Clave única de registro de propuesta</t>
   </si>
   <si>
-    <t>man_porpuesta</t>
+    <t>man_propuesta</t>
   </si>
   <si>
     <t>Nombre de la manzana propuesta</t>
@@ -234,7 +252,7 @@
     <t>SERVICIOS</t>
   </si>
   <si>
-    <t>id_servicio</t>
+    <t>id_servicios</t>
   </si>
   <si>
     <t>Clave única de registro del servicio.</t>
@@ -276,53 +294,57 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18.0"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font/>
-    <font>
-      <b/>
-      <sz val="14.0"/>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
-      <color rgb="FF000000"/>
-      <name val="Docs-Calibri"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="18.0"/>
+      <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="14.0"/>
+      <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="3">
@@ -330,7 +352,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -340,27 +362,39 @@
     </fill>
   </fills>
   <borders count="5">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -370,6 +404,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -384,61 +419,59 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+  <cellXfs count="11">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="4" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -628,744 +661,746 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:E1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="D75" sqref="D75"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="10.71"/>
-    <col customWidth="1" min="2" max="2" width="24.43"/>
-    <col customWidth="1" min="3" max="3" width="10.86"/>
-    <col customWidth="1" min="4" max="4" width="17.71"/>
-    <col customWidth="1" min="5" max="5" width="44.86"/>
-    <col customWidth="1" min="6" max="6" width="13.14"/>
-    <col customWidth="1" min="7" max="26" width="10.71"/>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="44.85546875" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="7" max="26" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="2:5">
+      <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3">
-      <c r="B3" s="4" t="s">
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="10"/>
+    </row>
+    <row r="3" spans="2:5">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4">
-      <c r="B4" s="5" t="s">
+    <row r="4" spans="2:5">
+      <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="5">
-        <v>11.0</v>
-      </c>
-      <c r="D4" s="5" t="s">
+      <c r="C4" s="2">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5">
-      <c r="B5" s="5" t="s">
+    <row r="5" spans="2:5">
+      <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="5">
-        <v>30.0</v>
-      </c>
-      <c r="D5" s="5" t="s">
+      <c r="C5" s="2">
+        <v>30</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6">
-      <c r="B6" s="5" t="s">
+    <row r="6" spans="2:5">
+      <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="5">
-        <v>30.0</v>
-      </c>
-      <c r="D6" s="5" t="s">
+      <c r="C6" s="2">
+        <v>30</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7">
-      <c r="B7" s="5" t="s">
+    <row r="7" spans="2:5">
+      <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="6">
-        <v>50.0</v>
-      </c>
-      <c r="D7" s="5" t="s">
+      <c r="C7" s="2">
+        <v>50</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8">
-      <c r="B8" s="6" t="s">
+    <row r="8" spans="2:5">
+      <c r="B8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="6">
-        <v>11.0</v>
-      </c>
-      <c r="D8" s="5" t="s">
+      <c r="C8" s="2">
+        <v>11</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12">
-      <c r="B12" s="1" t="s">
+    <row r="12" spans="2:5">
+      <c r="B12" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13">
-      <c r="B13" s="4" t="s">
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="10"/>
+    </row>
+    <row r="13" spans="2:5">
+      <c r="B13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14">
-      <c r="B14" s="5" t="s">
+    <row r="14" spans="2:5">
+      <c r="B14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="5">
-        <v>11.0</v>
-      </c>
-      <c r="D14" s="5" t="s">
+      <c r="C14" s="2">
+        <v>11</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15">
-      <c r="B15" s="5" t="s">
+    <row r="15" spans="2:5">
+      <c r="B15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="5">
-        <v>30.0</v>
-      </c>
-      <c r="D15" s="5" t="s">
+      <c r="C15" s="2">
+        <v>30</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16">
-      <c r="B16" s="5" t="s">
+    <row r="16" spans="2:5">
+      <c r="B16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="5">
-        <v>30.0</v>
-      </c>
-      <c r="D16" s="5" t="s">
+      <c r="C16" s="2">
+        <v>30</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17">
-      <c r="B17" s="5" t="s">
+    <row r="17" spans="2:5">
+      <c r="B17" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="6">
-        <v>50.0</v>
-      </c>
-      <c r="D17" s="5" t="s">
+      <c r="C17" s="2">
+        <v>50</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18">
-      <c r="B18" s="6" t="s">
+    <row r="18" spans="2:5">
+      <c r="B18" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="6">
-        <v>11.0</v>
-      </c>
-      <c r="D18" s="5" t="s">
+      <c r="C18" s="2">
+        <v>11</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="19">
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-    </row>
-    <row r="21" ht="15.75" customHeight="1"/>
-    <row r="22" ht="15.75" customHeight="1">
-      <c r="B22" s="1" t="s">
+    <row r="19" spans="2:5">
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+    </row>
+    <row r="21" spans="2:5" ht="15.75" customHeight="1"/>
+    <row r="22" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B22" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="3"/>
-    </row>
-    <row r="23" ht="15.75" customHeight="1">
-      <c r="B23" s="4" t="s">
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="10"/>
+    </row>
+    <row r="23" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B23" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="24" ht="15.75" customHeight="1">
-      <c r="B24" s="6" t="s">
+    <row r="24" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B24" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="6">
-        <v>19.0</v>
-      </c>
-      <c r="D24" s="6" t="s">
+      <c r="C24" s="2">
+        <v>19</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="E24" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="25" ht="15.75" customHeight="1">
-      <c r="B25" s="6" t="s">
+    <row r="25" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B25" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="6">
-        <v>5.0</v>
-      </c>
-      <c r="D25" s="5" t="s">
+      <c r="C25" s="2">
+        <v>30</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="E25" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="26" ht="15.75" customHeight="1">
-      <c r="B26" s="5" t="s">
+    <row r="26" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B26" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C26" s="5">
-        <v>30.0</v>
-      </c>
-      <c r="D26" s="5" t="s">
+      <c r="C26" s="2">
+        <v>30</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="E26" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="27" ht="15.75" customHeight="1">
-      <c r="B27" s="5" t="s">
+    <row r="27" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B27" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="5">
-        <v>30.0</v>
-      </c>
-      <c r="D27" s="5" t="s">
+      <c r="C27" s="2">
+        <v>30</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="E27" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="28" ht="15.75" customHeight="1">
-      <c r="B28" s="5" t="s">
+    <row r="28" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B28" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C28" s="5">
-        <v>20.0</v>
-      </c>
-      <c r="D28" s="5" t="s">
+      <c r="C28" s="2">
+        <v>20</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="E28" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="29" ht="15.75" customHeight="1">
-      <c r="B29" s="5" t="s">
+    <row r="29" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B29" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C29" s="5">
-        <v>50.0</v>
-      </c>
-      <c r="D29" s="5" t="s">
+      <c r="C29" s="2">
+        <v>50</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="E29" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="30" ht="15.75" customHeight="1">
-      <c r="B30" s="5" t="s">
+    <row r="30" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B30" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C30" s="5">
-        <v>40.0</v>
-      </c>
-      <c r="D30" s="5" t="s">
+      <c r="C30" s="2">
+        <v>40</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="E30" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="31" ht="15.75" customHeight="1">
-      <c r="B31" s="5" t="s">
+    <row r="31" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B31" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C31" s="5">
-        <v>20.0</v>
-      </c>
-      <c r="D31" s="5" t="s">
+      <c r="C31" s="2">
+        <v>20</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E31" s="5" t="s">
+      <c r="E31" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="32" ht="15.75" customHeight="1">
-      <c r="B32" s="5" t="s">
+    <row r="32" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B32" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C32" s="6">
-        <v>50.0</v>
-      </c>
-      <c r="D32" s="5" t="s">
+      <c r="C32" s="2">
+        <v>50</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E32" s="5" t="s">
+      <c r="E32" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="33" ht="15.75" customHeight="1">
-      <c r="B33" s="5" t="s">
+    <row r="33" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B33" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C33" s="6">
-        <v>40.0</v>
-      </c>
-      <c r="D33" s="5" t="s">
+      <c r="C33" s="2">
+        <v>40</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E33" s="5" t="s">
+      <c r="E33" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="34" ht="15.75" customHeight="1"/>
-    <row r="35" ht="15.75" customHeight="1"/>
-    <row r="36" ht="15.75" customHeight="1"/>
-    <row r="37" ht="15.75" customHeight="1">
-      <c r="B37" s="1" t="s">
+    <row r="34" spans="2:5" ht="15.75" customHeight="1"/>
+    <row r="35" spans="2:5" ht="15.75" customHeight="1"/>
+    <row r="36" spans="2:5" ht="15.75" customHeight="1"/>
+    <row r="37" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B37" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="3"/>
-    </row>
-    <row r="38" ht="15.75" customHeight="1">
-      <c r="B38" s="4" t="s">
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="10"/>
+    </row>
+    <row r="38" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B38" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C38" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D38" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E38" s="4" t="s">
+      <c r="E38" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="39" ht="15.75" customHeight="1">
-      <c r="B39" s="5" t="s">
+    <row r="39" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B39" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C39" s="6">
-        <v>11.0</v>
-      </c>
-      <c r="D39" s="5" t="s">
+      <c r="C39" s="2">
+        <v>11</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E39" s="5" t="s">
+      <c r="E39" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="40" ht="15.75" customHeight="1">
-      <c r="B40" s="6" t="s">
+    <row r="40" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B40" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C40" s="6">
-        <v>11.0</v>
-      </c>
-      <c r="D40" s="5" t="s">
+      <c r="C40" s="2">
+        <v>11</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E40" s="5" t="s">
+      <c r="E40" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="41" ht="15.75" customHeight="1">
-      <c r="B41" s="7"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-    </row>
-    <row r="42" ht="15.75" customHeight="1">
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-    </row>
-    <row r="43" ht="15.75" customHeight="1"/>
-    <row r="44" ht="15.75" customHeight="1">
-      <c r="B44" s="1" t="s">
+    <row r="41" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+    </row>
+    <row r="42" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+    </row>
+    <row r="43" spans="2:5" ht="15.75" customHeight="1"/>
+    <row r="44" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B44" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="3"/>
-    </row>
-    <row r="45" ht="15.75" customHeight="1">
-      <c r="B45" s="4" t="s">
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="10"/>
+    </row>
+    <row r="45" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B45" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="C45" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D45" s="4" t="s">
+      <c r="D45" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E45" s="4" t="s">
+      <c r="E45" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="46" ht="15.75" customHeight="1">
-      <c r="B46" s="5" t="s">
+    <row r="46" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B46" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C46" s="5">
-        <v>11.0</v>
-      </c>
-      <c r="D46" s="5" t="s">
+      <c r="C46" s="2">
+        <v>11</v>
+      </c>
+      <c r="D46" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E46" s="5" t="s">
+      <c r="E46" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="47" ht="15.75" customHeight="1">
-      <c r="B47" s="6" t="s">
+    <row r="47" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B47" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C47" s="5">
-        <v>30.0</v>
-      </c>
-      <c r="D47" s="5" t="s">
+      <c r="C47" s="2">
+        <v>30</v>
+      </c>
+      <c r="D47" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E47" s="5" t="s">
+      <c r="E47" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="48" ht="15.75" customHeight="1"/>
-    <row r="49" ht="15.75" customHeight="1"/>
-    <row r="50" ht="15.75" customHeight="1"/>
-    <row r="51" ht="15.75" customHeight="1">
-      <c r="B51" s="1" t="s">
+    <row r="48" spans="2:5" ht="15.75" customHeight="1"/>
+    <row r="49" spans="2:5" ht="15.75" customHeight="1"/>
+    <row r="50" spans="2:5" ht="15.75" customHeight="1"/>
+    <row r="51" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B51" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-      <c r="E51" s="3"/>
-    </row>
-    <row r="52" ht="15.75" customHeight="1">
-      <c r="B52" s="4" t="s">
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="10"/>
+    </row>
+    <row r="52" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B52" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="C52" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D52" s="4" t="s">
+      <c r="D52" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E52" s="4" t="s">
+      <c r="E52" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="53" ht="15.75" customHeight="1">
-      <c r="B53" s="5" t="s">
+    <row r="53" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B53" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C53" s="5">
-        <v>11.0</v>
-      </c>
-      <c r="D53" s="5" t="s">
+      <c r="C53" s="2">
+        <v>11</v>
+      </c>
+      <c r="D53" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E53" s="5" t="s">
+      <c r="E53" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="54" ht="15.75" customHeight="1">
-      <c r="B54" s="5" t="s">
+    <row r="54" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B54" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C54" s="5">
-        <v>30.0</v>
-      </c>
-      <c r="D54" s="5" t="s">
+      <c r="C54" s="2">
+        <v>30</v>
+      </c>
+      <c r="D54" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E54" s="5" t="s">
+      <c r="E54" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="55" ht="15.75" customHeight="1">
-      <c r="B55" s="5" t="s">
+    <row r="55" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B55" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C55" s="6">
-        <v>30.0</v>
-      </c>
-      <c r="D55" s="5" t="s">
+      <c r="C55" s="2">
+        <v>30</v>
+      </c>
+      <c r="D55" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E55" s="5" t="s">
+      <c r="E55" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="56" ht="15.75" customHeight="1">
-      <c r="B56" s="5" t="s">
+    <row r="56" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B56" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C56" s="5"/>
-      <c r="D56" s="5" t="s">
+      <c r="C56" s="2"/>
+      <c r="D56" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E56" s="5" t="s">
+      <c r="E56" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="57" ht="15.75" customHeight="1">
-      <c r="B57" s="8" t="s">
+    <row r="57" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B57" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C57" s="6">
-        <v>19.0</v>
-      </c>
-      <c r="D57" s="6" t="s">
+      <c r="C57" s="2">
+        <v>19</v>
+      </c>
+      <c r="D57" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E57" s="5" t="s">
+      <c r="E57" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="58" ht="15.75" customHeight="1"/>
-    <row r="59" ht="15.75" customHeight="1"/>
-    <row r="60" ht="15.75" customHeight="1"/>
-    <row r="61" ht="15.75" customHeight="1">
-      <c r="B61" s="9" t="s">
+    <row r="58" spans="2:5" ht="15.75" customHeight="1"/>
+    <row r="59" spans="2:5" ht="15.75" customHeight="1"/>
+    <row r="60" spans="2:5" ht="15.75" customHeight="1"/>
+    <row r="61" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B61" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="C61" s="2"/>
-      <c r="D61" s="2"/>
-      <c r="E61" s="3"/>
-    </row>
-    <row r="62" ht="15.75" customHeight="1">
-      <c r="B62" s="10" t="s">
+      <c r="C61" s="9"/>
+      <c r="D61" s="9"/>
+      <c r="E61" s="10"/>
+    </row>
+    <row r="62" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B62" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C62" s="10" t="s">
+      <c r="C62" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D62" s="10" t="s">
+      <c r="D62" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E62" s="10" t="s">
+      <c r="E62" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="63" ht="15.75" customHeight="1">
-      <c r="B63" s="11" t="s">
+    <row r="63" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B63" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C63" s="11">
-        <v>11.0</v>
-      </c>
-      <c r="D63" s="11" t="s">
+      <c r="C63" s="5">
+        <v>11</v>
+      </c>
+      <c r="D63" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E63" s="11" t="s">
+      <c r="E63" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="64" ht="15.75" customHeight="1">
-      <c r="B64" s="12" t="s">
+    <row r="64" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B64" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C64" s="11">
-        <v>30.0</v>
-      </c>
-      <c r="D64" s="11" t="s">
+      <c r="C64" s="5">
+        <v>30</v>
+      </c>
+      <c r="D64" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E64" s="11" t="s">
+      <c r="E64" s="5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="65" ht="15.75" customHeight="1">
-      <c r="B65" s="6" t="s">
+    <row r="65" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B65" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C65" s="5">
-        <v>100.0</v>
-      </c>
-      <c r="D65" s="5" t="s">
+      <c r="C65" s="2">
+        <v>100</v>
+      </c>
+      <c r="D65" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E65" s="5" t="s">
+      <c r="E65" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="66" ht="15.75" customHeight="1">
-      <c r="B66" s="6" t="s">
+    <row r="66" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B66" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C66" s="6">
-        <v>50.0</v>
-      </c>
-      <c r="D66" s="5" t="s">
+      <c r="C66" s="2">
+        <v>50</v>
+      </c>
+      <c r="D66" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E66" s="5" t="s">
+      <c r="E66" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="67" ht="15.75" customHeight="1">
-      <c r="B67" s="6" t="s">
+    <row r="67" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B67" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C67" s="6">
-        <v>50.0</v>
-      </c>
-      <c r="D67" s="5" t="s">
+      <c r="C67" s="2">
+        <v>50</v>
+      </c>
+      <c r="D67" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E67" s="5" t="s">
+      <c r="E67" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="68" ht="15.75" customHeight="1"/>
-    <row r="69" ht="15.75" customHeight="1"/>
-    <row r="70" ht="15.75" customHeight="1"/>
-    <row r="71" ht="15.75" customHeight="1">
-      <c r="B71" s="1" t="s">
+    <row r="68" spans="2:5" ht="15.75" customHeight="1"/>
+    <row r="69" spans="2:5" ht="15.75" customHeight="1"/>
+    <row r="70" spans="2:5" ht="15.75" customHeight="1"/>
+    <row r="71" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B71" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="C71" s="2"/>
-      <c r="D71" s="2"/>
-      <c r="E71" s="3"/>
-    </row>
-    <row r="72" ht="15.75" customHeight="1">
-      <c r="B72" s="4" t="s">
+      <c r="C71" s="9"/>
+      <c r="D71" s="9"/>
+      <c r="E71" s="10"/>
+    </row>
+    <row r="72" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B72" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C72" s="4" t="s">
+      <c r="C72" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D72" s="4" t="s">
+      <c r="D72" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E72" s="4" t="s">
+      <c r="E72" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="73" ht="15.75" customHeight="1">
-      <c r="B73" s="5" t="s">
+    <row r="73" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B73" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C73" s="5">
-        <v>11.0</v>
-      </c>
-      <c r="D73" s="5" t="s">
+      <c r="C73" s="2">
+        <v>11</v>
+      </c>
+      <c r="D73" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E73" s="5" t="s">
+      <c r="E73" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="74" ht="15.75" customHeight="1">
-      <c r="B74" s="6" t="s">
+    <row r="74" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B74" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C74" s="5">
-        <v>11.0</v>
-      </c>
-      <c r="D74" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E74" s="5" t="s">
+      <c r="C74" s="2">
+        <v>19</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E74" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="75" ht="15.75" customHeight="1"/>
-    <row r="76" ht="15.75" customHeight="1"/>
-    <row r="77" ht="15.75" customHeight="1"/>
-    <row r="78" ht="15.75" customHeight="1"/>
-    <row r="79" ht="15.75" customHeight="1"/>
-    <row r="80" ht="15.75" customHeight="1"/>
+    <row r="75" spans="2:5" ht="15.75" customHeight="1"/>
+    <row r="76" spans="2:5" ht="15.75" customHeight="1"/>
+    <row r="77" spans="2:5" ht="15.75" customHeight="1"/>
+    <row r="78" spans="2:5" ht="15.75" customHeight="1"/>
+    <row r="79" spans="2:5" ht="15.75" customHeight="1"/>
+    <row r="80" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="81" ht="15.75" customHeight="1"/>
     <row r="82" ht="15.75" customHeight="1"/>
     <row r="83" ht="15.75" customHeight="1"/>
@@ -2288,18 +2323,16 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="B51:E51"/>
+    <mergeCell ref="B61:E61"/>
+    <mergeCell ref="B71:E71"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="B22:E22"/>
     <mergeCell ref="B37:E37"/>
     <mergeCell ref="B44:E44"/>
-    <mergeCell ref="B51:E51"/>
-    <mergeCell ref="B61:E61"/>
-    <mergeCell ref="B71:E71"/>
   </mergeCells>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Base de datos 3
</commit_message>
<xml_diff>
--- a/ddbb/diccionario_datos.xlsx
+++ b/ddbb/diccionario_datos.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27004"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0453ED16-2495-4225-ABD9-BFE899792768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DFA41029-AA00-45D2-9642-4C332253F987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="87">
   <si>
     <t>ESTABLECIMIENTO</t>
   </si>
@@ -184,6 +184,12 @@
   </si>
   <si>
     <t>Ocupación de la mujer cuidadora.</t>
+  </si>
+  <si>
+    <t>rol_mujer</t>
+  </si>
+  <si>
+    <t>Rol otorgado tanto a usuario como administrador.</t>
   </si>
   <si>
     <t>MANZANAS_SERVICIOS</t>
@@ -361,7 +367,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -421,11 +427,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -450,6 +469,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -668,10 +690,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:E1000"/>
+  <dimension ref="B2:E1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="D75" sqref="D75"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -689,9 +711,9 @@
       <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="11"/>
     </row>
     <row r="3" spans="2:5">
       <c r="B3" s="1" t="s">
@@ -781,9 +803,9 @@
       <c r="B12" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="11"/>
     </row>
     <row r="13" spans="2:5">
       <c r="B13" s="1" t="s">
@@ -880,9 +902,9 @@
       <c r="B22" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="11"/>
     </row>
     <row r="23" spans="2:5" ht="15.75" customHeight="1">
       <c r="B23" s="1" t="s">
@@ -1025,61 +1047,61 @@
       </c>
     </row>
     <row r="33" spans="2:5" ht="15.75" customHeight="1">
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33" s="9">
         <v>40</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D33" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="E33" s="9" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="2:5" ht="15.75" customHeight="1"/>
+    <row r="34" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B34" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C34" s="2">
+        <v>30</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
     <row r="35" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="36" spans="2:5" ht="15.75" customHeight="1"/>
-    <row r="37" spans="2:5" ht="15.75" customHeight="1">
-      <c r="B37" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="10"/>
-    </row>
+    <row r="37" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="38" spans="2:5" ht="15.75" customHeight="1">
-      <c r="B38" s="1" t="s">
+      <c r="B38" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="11"/>
+    </row>
+    <row r="39" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B39" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C39" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D39" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E39" s="1" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" ht="15.75" customHeight="1">
-      <c r="B39" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C39" s="2">
-        <v>11</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="40" spans="2:5" ht="15.75" customHeight="1">
       <c r="B40" s="2" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="C40" s="2">
         <v>11</v>
@@ -1088,14 +1110,22 @@
         <v>6</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41" spans="2:5" ht="15.75" customHeight="1">
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
+      <c r="B41" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C41" s="2">
+        <v>11</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="42" spans="2:5" ht="15.75" customHeight="1">
       <c r="B42" s="3"/>
@@ -1103,41 +1133,33 @@
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
     </row>
-    <row r="43" spans="2:5" ht="15.75" customHeight="1"/>
-    <row r="44" spans="2:5" ht="15.75" customHeight="1">
-      <c r="B44" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C44" s="9"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="10"/>
-    </row>
+    <row r="43" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+    </row>
+    <row r="44" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="45" spans="2:5" ht="15.75" customHeight="1">
-      <c r="B45" s="1" t="s">
+      <c r="B45" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="11"/>
+    </row>
+    <row r="46" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B46" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C46" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D46" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="E46" s="1" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="46" spans="2:5" ht="15.75" customHeight="1">
-      <c r="B46" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C46" s="2">
-        <v>11</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="47" spans="2:5" ht="15.75" customHeight="1">
@@ -1145,52 +1167,52 @@
         <v>57</v>
       </c>
       <c r="C47" s="2">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="48" spans="2:5" ht="15.75" customHeight="1"/>
+    <row r="48" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B48" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C48" s="2">
+        <v>30</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
     <row r="49" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="50" spans="2:5" ht="15.75" customHeight="1"/>
-    <row r="51" spans="2:5" ht="15.75" customHeight="1">
-      <c r="B51" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C51" s="9"/>
-      <c r="D51" s="9"/>
-      <c r="E51" s="10"/>
-    </row>
+    <row r="51" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="52" spans="2:5" ht="15.75" customHeight="1">
-      <c r="B52" s="1" t="s">
+      <c r="B52" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C52" s="10"/>
+      <c r="D52" s="10"/>
+      <c r="E52" s="11"/>
+    </row>
+    <row r="53" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B53" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C53" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="D53" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E52" s="1" t="s">
+      <c r="E53" s="1" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="53" spans="2:5" ht="15.75" customHeight="1">
-      <c r="B53" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C53" s="2">
-        <v>11</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="54" spans="2:5" ht="15.75" customHeight="1">
@@ -1198,10 +1220,10 @@
         <v>62</v>
       </c>
       <c r="C54" s="2">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>63</v>
@@ -1225,65 +1247,65 @@
       <c r="B56" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C56" s="2"/>
+      <c r="C56" s="2">
+        <v>30</v>
+      </c>
       <c r="D56" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E56" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E56" s="2" t="s">
+    </row>
+    <row r="57" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B57" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="57" spans="2:5" ht="15.75" customHeight="1">
-      <c r="B57" s="6" t="s">
+      <c r="C57" s="2"/>
+      <c r="D57" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="C57" s="2">
-        <v>19</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="58" spans="2:5" ht="15.75" customHeight="1"/>
+    <row r="58" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B58" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C58" s="2">
+        <v>19</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
     <row r="59" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="60" spans="2:5" ht="15.75" customHeight="1"/>
-    <row r="61" spans="2:5" ht="15.75" customHeight="1">
-      <c r="B61" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="C61" s="9"/>
-      <c r="D61" s="9"/>
-      <c r="E61" s="10"/>
-    </row>
+    <row r="61" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="62" spans="2:5" ht="15.75" customHeight="1">
-      <c r="B62" s="4" t="s">
+      <c r="B62" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C62" s="10"/>
+      <c r="D62" s="10"/>
+      <c r="E62" s="11"/>
+    </row>
+    <row r="63" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B63" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C62" s="4" t="s">
+      <c r="C63" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D62" s="4" t="s">
+      <c r="D63" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E62" s="4" t="s">
+      <c r="E63" s="4" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="63" spans="2:5" ht="15.75" customHeight="1">
-      <c r="B63" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C63" s="5">
-        <v>11</v>
-      </c>
-      <c r="D63" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E63" s="5" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="64" spans="2:5" ht="15.75" customHeight="1">
@@ -1291,26 +1313,26 @@
         <v>74</v>
       </c>
       <c r="C64" s="5">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E64" s="5" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="65" spans="2:5" ht="15.75" customHeight="1">
-      <c r="B65" s="2" t="s">
+      <c r="B65" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C65" s="2">
-        <v>100</v>
-      </c>
-      <c r="D65" s="2" t="s">
+      <c r="C65" s="5">
+        <v>30</v>
+      </c>
+      <c r="D65" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E65" s="2" t="s">
+      <c r="E65" s="5" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1319,7 +1341,7 @@
         <v>78</v>
       </c>
       <c r="C66" s="2">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>9</v>
@@ -1342,60 +1364,73 @@
         <v>81</v>
       </c>
     </row>
-    <row r="68" spans="2:5" ht="15.75" customHeight="1"/>
+    <row r="68" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B68" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C68" s="2">
+        <v>50</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
     <row r="69" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="70" spans="2:5" ht="15.75" customHeight="1"/>
-    <row r="71" spans="2:5" ht="15.75" customHeight="1">
-      <c r="B71" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C71" s="9"/>
-      <c r="D71" s="9"/>
-      <c r="E71" s="10"/>
-    </row>
+    <row r="71" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="72" spans="2:5" ht="15.75" customHeight="1">
-      <c r="B72" s="1" t="s">
+      <c r="B72" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C72" s="10"/>
+      <c r="D72" s="10"/>
+      <c r="E72" s="11"/>
+    </row>
+    <row r="73" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B73" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="C73" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D72" s="1" t="s">
+      <c r="D73" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E72" s="1" t="s">
+      <c r="E73" s="1" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="73" spans="2:5" ht="15.75" customHeight="1">
-      <c r="B73" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C73" s="2">
-        <v>11</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E73" s="2" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="74" spans="2:5" ht="15.75" customHeight="1">
       <c r="B74" s="2" t="s">
-        <v>69</v>
+        <v>15</v>
       </c>
       <c r="C74" s="2">
+        <v>11</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="75" spans="2:5" ht="15.75" customHeight="1">
+      <c r="B75" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C75" s="2">
         <v>19</v>
       </c>
-      <c r="D74" s="2" t="s">
+      <c r="D75" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E74" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="75" spans="2:5" ht="15.75" customHeight="1"/>
+      <c r="E75" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
     <row r="76" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="77" spans="2:5" ht="15.75" customHeight="1"/>
     <row r="78" spans="2:5" ht="15.75" customHeight="1"/>
@@ -2321,16 +2356,17 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="1001" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="B51:E51"/>
-    <mergeCell ref="B61:E61"/>
-    <mergeCell ref="B71:E71"/>
+    <mergeCell ref="B52:E52"/>
+    <mergeCell ref="B62:E62"/>
+    <mergeCell ref="B72:E72"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B37:E37"/>
-    <mergeCell ref="B44:E44"/>
+    <mergeCell ref="B38:E38"/>
+    <mergeCell ref="B45:E45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>